<commit_message>
modify the file structure
</commit_message>
<xml_diff>
--- a/source/品势对战表/品势标准输入.xlsx
+++ b/source/品势对战表/品势标准输入.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wtf\WTF-Trans\WTF\source\品势对战表\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2097CE8-E1EE-4F96-BA34-288EBC66B3C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388A283C-1481-44F6-A38B-63420D166DB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="44">
   <si>
     <t>场次</t>
   </si>
@@ -155,6 +155,10 @@
   </si>
   <si>
     <t>太极三章;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小学甲组男中级</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -511,7 +515,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -835,7 +839,7 @@
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>11</v>

</xml_diff>